<commit_message>
plan de cuentas, asientos empezados
</commit_message>
<xml_diff>
--- a/Aplicación/AuditoriaProvincias.xlsx
+++ b/Aplicación/AuditoriaProvincias.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>Id Provincia</t>
   </si>
@@ -35,79 +35,76 @@
     <t>Nick</t>
   </si>
   <si>
-    <t>Nuevas Provincias</t>
-  </si>
-  <si>
-    <t>2019-06-03 18:46:11.0</t>
-  </si>
-  <si>
-    <t>10.10.10.131</t>
+    <t>Nueva provincia</t>
+  </si>
+  <si>
+    <t>2019-06-01 20:01:58.0</t>
+  </si>
+  <si>
+    <t>192.168.1.20</t>
+  </si>
+  <si>
+    <t>Eliminacion</t>
+  </si>
+  <si>
+    <t>emi</t>
+  </si>
+  <si>
+    <t>Jujuy</t>
+  </si>
+  <si>
+    <t>2019-06-01 20:01:50.0</t>
   </si>
   <si>
     <t>Modificacion</t>
   </si>
   <si>
-    <t>emi</t>
-  </si>
-  <si>
-    <t>Nuevas Provincia</t>
-  </si>
-  <si>
-    <t>2019-06-03 18:46:01.0</t>
-  </si>
-  <si>
-    <t>Nueva Provincia</t>
-  </si>
-  <si>
-    <t>2019-06-03 18:45:47.0</t>
+    <t>sevilla</t>
+  </si>
+  <si>
+    <t>2019-06-01 18:49:13.0</t>
+  </si>
+  <si>
+    <t>españas</t>
+  </si>
+  <si>
+    <t>2019-06-01 18:23:49.0</t>
+  </si>
+  <si>
+    <t>2019-06-01 18:16:49.0</t>
+  </si>
+  <si>
+    <t>asxas</t>
+  </si>
+  <si>
+    <t>2019-06-01 09:32:29.0</t>
+  </si>
+  <si>
+    <t>2019-06-01 09:32:26.0</t>
+  </si>
+  <si>
+    <t>dasdasd</t>
+  </si>
+  <si>
+    <t>2019-06-01 09:32:20.0</t>
   </si>
   <si>
     <t>Nueva</t>
   </si>
   <si>
-    <t>Corrientes</t>
-  </si>
-  <si>
-    <t>2019-06-03 15:10:14.0</t>
-  </si>
-  <si>
-    <t>192.168.0.167</t>
-  </si>
-  <si>
-    <t>Formosa</t>
-  </si>
-  <si>
-    <t>2019-06-03 15:10:06.0</t>
-  </si>
-  <si>
-    <t>Buenos Aires</t>
-  </si>
-  <si>
-    <t>2019-06-03 15:10:00.0</t>
-  </si>
-  <si>
-    <t>2019-06-02 23:51:15.0</t>
-  </si>
-  <si>
-    <t>Eliminacion</t>
-  </si>
-  <si>
-    <t>Formosaaaaa</t>
-  </si>
-  <si>
-    <t>2019-06-02 23:51:12.0</t>
-  </si>
-  <si>
-    <t>Chacos</t>
-  </si>
-  <si>
-    <t>2019-06-02 22:10:10.0</t>
-  </si>
-  <si>
-    <t>2019-06-02 22:04:34.0</t>
-  </si>
-  <si>
-    <t>2019-06-02 22:04:18.0</t>
+    <t>2019-05-30 21:54:01.0</t>
+  </si>
+  <si>
+    <t>192.168.26.219</t>
+  </si>
+  <si>
+    <t>2019-05-30 20:55:19.0</t>
+  </si>
+  <si>
+    <t>españa</t>
+  </si>
+  <si>
+    <t>2019-05-30 20:38:26.0</t>
   </si>
 </sst>
 </file>
@@ -159,9 +156,9 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="11.44921875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="17.1796875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="15.4765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="21.33984375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="13.8515625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.96875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="12.6484375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="10.15625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="4.890625" customWidth="true" bestFit="true"/>
@@ -192,7 +189,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>8.0</v>
+        <v>20.0</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -207,7 +204,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -215,7 +212,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>8.0</v>
+        <v>46.0</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -227,10 +224,10 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -238,22 +235,22 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>8.0</v>
+        <v>53.0</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -261,7 +258,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7.0</v>
+        <v>52.0</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -270,13 +267,13 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -284,22 +281,22 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6.0</v>
+        <v>52.0</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -307,22 +304,22 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5.0</v>
+        <v>54.0</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -330,22 +327,22 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.0</v>
+        <v>54.0</v>
       </c>
       <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -353,22 +350,22 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4.0</v>
+        <v>54.0</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
       </c>
       <c r="F9" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -376,22 +373,22 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3.0</v>
+        <v>52.0</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F10" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
@@ -399,22 +396,22 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4.0</v>
+        <v>53.0</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
@@ -422,22 +419,22 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>4.0</v>
+        <v>52.0</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F12" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>

</xml_diff>